<commit_message>
Added new entrances to excel and csv
Added entrances from Justins list to excel and csv
</commit_message>
<xml_diff>
--- a/src/qrStuff/entrance_urls_autofill.xlsx
+++ b/src/qrStuff/entrance_urls_autofill.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\benes\Desktop\CS 499 Hospital GPS\hospital-navigation\src\qrStuff\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{585F08A3-871C-4136-9BFC-4523B9CFEB07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F66543C4-F233-4478-B251-CA39439357FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{C76E6DE7-7D89-4428-B1DF-501A79B2B33E}"/>
   </bookViews>
@@ -33,14 +33,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>1st Floor Main Entrance</t>
   </si>
   <si>
-    <t>UHS Entrance</t>
-  </si>
-  <si>
     <t>South Limestone Entrance B</t>
   </si>
   <si>
@@ -53,7 +50,31 @@
     <t>2nd Floor Main Entrance</t>
   </si>
   <si>
-    <t>3rd Floor Main Entrance</t>
+    <t>Wing D North Parking Garage Entrance</t>
+  </si>
+  <si>
+    <t>University Health Services Entrance</t>
+  </si>
+  <si>
+    <t>Charles T. Wethington Building Entrance</t>
+  </si>
+  <si>
+    <t>University Health Services Bridge Entrance</t>
+  </si>
+  <si>
+    <t>A.B. Chandler Bridge Entrance</t>
+  </si>
+  <si>
+    <t>3rd Floor Parking Garage Entrance</t>
+  </si>
+  <si>
+    <t>4th Floor Parking Garage Entrance</t>
+  </si>
+  <si>
+    <t>5th Floor Parking Garage Entrance</t>
+  </si>
+  <si>
+    <t>s</t>
   </si>
 </sst>
 </file>
@@ -914,9 +935,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83D53554-6513-403D-AD2F-7C34FD05D68A}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:C13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -928,27 +951,27 @@
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="str">
         <f>_xlfn.CONCAT("https://hospitalnavigation.netlify.app/start/?start=",SUBSTITUTE(B1,".png",""))</f>
-        <v>https://hospitalnavigation.netlify.app/start/?start=1st_Floor_Main_Entrance</v>
+        <v>https://hospitalnavigation.netlify.app/start/?start=Wing_D_North_Parking_Garage_Entrance</v>
       </c>
       <c r="B1" t="str">
         <f>_xlfn.CONCAT(SUBSTITUTE(C1," ","_"),".png")</f>
-        <v>1st_Floor_Main_Entrance.png</v>
+        <v>Wing_D_North_Parking_Garage_Entrance.png</v>
       </c>
       <c r="C1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="str">
-        <f t="shared" ref="A2:A7" si="0">_xlfn.CONCAT("https://hospitalnavigation.netlify.app/start/?start=",SUBSTITUTE(B2,".png",""))</f>
-        <v>https://hospitalnavigation.netlify.app/start/?start=UHS_Entrance</v>
+        <f t="shared" ref="A2:A14" si="0">_xlfn.CONCAT("https://hospitalnavigation.netlify.app/start/?start=",SUBSTITUTE(B2,".png",""))</f>
+        <v>https://hospitalnavigation.netlify.app/start/?start=South_Limestone_Entrance_A</v>
       </c>
       <c r="B2" t="str">
-        <f t="shared" ref="B2:B7" si="1">_xlfn.CONCAT(SUBSTITUTE(C2," ","_"),".png")</f>
-        <v>UHS_Entrance.png</v>
+        <f>_xlfn.CONCAT(SUBSTITUTE(C2," ","_"),".png")</f>
+        <v>South_Limestone_Entrance_A.png</v>
       </c>
       <c r="C2" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -957,11 +980,11 @@
         <v>https://hospitalnavigation.netlify.app/start/?start=South_Limestone_Entrance_B</v>
       </c>
       <c r="B3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="B3:B14" si="1">_xlfn.CONCAT(SUBSTITUTE(C3," ","_"),".png")</f>
         <v>South_Limestone_Entrance_B.png</v>
       </c>
       <c r="C3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -970,7 +993,7 @@
         <v>https://hospitalnavigation.netlify.app/start/?start=South_Limestone_Entrance_A</v>
       </c>
       <c r="B4" t="str">
-        <f t="shared" si="1"/>
+        <f>_xlfn.CONCAT(SUBSTITUTE(C2," ","_"),".png")</f>
         <v>South_Limestone_Entrance_A.png</v>
       </c>
       <c r="C4" t="s">
@@ -983,37 +1006,120 @@
         <v>https://hospitalnavigation.netlify.app/start/?start=Rose_Street_Entrance</v>
       </c>
       <c r="B5" t="str">
-        <f t="shared" si="1"/>
+        <f>_xlfn.CONCAT(SUBSTITUTE(C4," ","_"),".png")</f>
         <v>Rose_Street_Entrance.png</v>
       </c>
       <c r="C5" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="str">
         <f t="shared" si="0"/>
-        <v>https://hospitalnavigation.netlify.app/start/?start=2nd_Floor_Main_Entrance</v>
+        <v>https://hospitalnavigation.netlify.app/start/?start=1st_Floor_Main_Entrance</v>
       </c>
       <c r="B6" t="str">
         <f t="shared" si="1"/>
-        <v>2nd_Floor_Main_Entrance.png</v>
+        <v>1st_Floor_Main_Entrance.png</v>
       </c>
       <c r="C6" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="str">
         <f t="shared" si="0"/>
-        <v>https://hospitalnavigation.netlify.app/start/?start=3rd_Floor_Main_Entrance</v>
+        <v>https://hospitalnavigation.netlify.app/start/?start=Charles_T._Wethington_Building_Entrance</v>
       </c>
       <c r="B7" t="str">
         <f t="shared" si="1"/>
-        <v>3rd_Floor_Main_Entrance.png</v>
+        <v>Charles_T._Wethington_Building_Entrance.png</v>
       </c>
       <c r="C7" t="s">
-        <v>6</v>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="str">
+        <f t="shared" si="0"/>
+        <v>https://hospitalnavigation.netlify.app/start/?start=2nd_Floor_Main_Entrance</v>
+      </c>
+      <c r="B8" t="str">
+        <f t="shared" si="1"/>
+        <v>2nd_Floor_Main_Entrance.png</v>
+      </c>
+      <c r="C8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="str">
+        <f t="shared" si="0"/>
+        <v>https://hospitalnavigation.netlify.app/start/?start=University_Health_Services_Bridge_Entrance</v>
+      </c>
+      <c r="B9" t="str">
+        <f t="shared" si="1"/>
+        <v>University_Health_Services_Bridge_Entrance.png</v>
+      </c>
+      <c r="C9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="str">
+        <f t="shared" si="0"/>
+        <v>https://hospitalnavigation.netlify.app/start/?start=A.B._Chandler_Bridge_Entrance</v>
+      </c>
+      <c r="B10" t="str">
+        <f t="shared" si="1"/>
+        <v>A.B._Chandler_Bridge_Entrance.png</v>
+      </c>
+      <c r="C10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="str">
+        <f t="shared" si="0"/>
+        <v>https://hospitalnavigation.netlify.app/start/?start=3rd_Floor_Parking_Garage_Entrance</v>
+      </c>
+      <c r="B11" t="str">
+        <f t="shared" si="1"/>
+        <v>3rd_Floor_Parking_Garage_Entrance.png</v>
+      </c>
+      <c r="C11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="str">
+        <f t="shared" si="0"/>
+        <v>https://hospitalnavigation.netlify.app/start/?start=4th_Floor_Parking_Garage_Entrance</v>
+      </c>
+      <c r="B12" t="str">
+        <f t="shared" si="1"/>
+        <v>4th_Floor_Parking_Garage_Entrance.png</v>
+      </c>
+      <c r="C12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="str">
+        <f t="shared" si="0"/>
+        <v>https://hospitalnavigation.netlify.app/start/?start=5th_Floor_Parking_Garage_Entrance</v>
+      </c>
+      <c r="B13" t="str">
+        <f t="shared" si="1"/>
+        <v>5th_Floor_Parking_Garage_Entrance.png</v>
+      </c>
+      <c r="C13" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update qr codes to use new URL
'I hope this is the last time' lol. Updated qrcode links to use new netlify URL.
</commit_message>
<xml_diff>
--- a/src/qrStuff/entrance_urls_autofill.xlsx
+++ b/src/qrStuff/entrance_urls_autofill.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\benes\Desktop\CS 499 Hospital GPS\hospital-navigation\src\qrStuff\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F997F9C9-ACB5-4B8E-AB57-51D9FCF9E29F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69DB4697-3879-49A5-9560-8093C304303B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{C76E6DE7-7D89-4428-B1DF-501A79B2B33E}"/>
   </bookViews>
@@ -1095,7 +1095,7 @@
   <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1107,8 +1107,8 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="str">
-        <f>_xlfn.CONCAT("https://hospitalnavigation.netlify.app/start/?start=",SUBSTITUTE(B1,".png",""))</f>
-        <v>https://hospitalnavigation.netlify.app/start/?start=5th_Floor_Parking_Garage_Entrance</v>
+        <f>_xlfn.CONCAT("https://uky-hospital-gps.netlify.app/start/?start=",SUBSTITUTE(B1,".png",""))</f>
+        <v>https://uky-hospital-gps.netlify.app/start/?start=5th_Floor_Parking_Garage_Entrance</v>
       </c>
       <c r="B1" t="str">
         <f>_xlfn.CONCAT(SUBSTITUTE(C1," ","_"),".png")</f>
@@ -1120,8 +1120,8 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="str">
-        <f t="shared" ref="A2:A13" si="0">_xlfn.CONCAT("https://hospitalnavigation.netlify.app/start/?start=",SUBSTITUTE(B2,".png",""))</f>
-        <v>https://hospitalnavigation.netlify.app/start/?start=4th_Floor_Parking_Garage_Entrance</v>
+        <f t="shared" ref="A2:A13" si="0">_xlfn.CONCAT("https://uky-hospital-gps.netlify.app/start/?start=",SUBSTITUTE(B2,".png",""))</f>
+        <v>https://uky-hospital-gps.netlify.app/start/?start=4th_Floor_Parking_Garage_Entrance</v>
       </c>
       <c r="B2" t="str">
         <f>_xlfn.CONCAT(SUBSTITUTE(C2," ","_"),".png")</f>
@@ -1134,7 +1134,7 @@
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="str">
         <f t="shared" si="0"/>
-        <v>https://hospitalnavigation.netlify.app/start/?start=3rd_Floor_Parking_Garage_Entrance</v>
+        <v>https://uky-hospital-gps.netlify.app/start/?start=3rd_Floor_Parking_Garage_Entrance</v>
       </c>
       <c r="B3" t="str">
         <f t="shared" ref="B3:B13" si="1">_xlfn.CONCAT(SUBSTITUTE(C3," ","_"),".png")</f>
@@ -1147,7 +1147,7 @@
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="str">
         <f t="shared" si="0"/>
-        <v>https://hospitalnavigation.netlify.app/start/?start=4th_Floor_Parking_Garage_Entrance</v>
+        <v>https://uky-hospital-gps.netlify.app/start/?start=4th_Floor_Parking_Garage_Entrance</v>
       </c>
       <c r="B4" t="str">
         <f>_xlfn.CONCAT(SUBSTITUTE(C2," ","_"),".png")</f>
@@ -1160,7 +1160,7 @@
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="str">
         <f t="shared" si="0"/>
-        <v>https://hospitalnavigation.netlify.app/start/?start=2nd_Floor_Parking_Garage_Entrance</v>
+        <v>https://uky-hospital-gps.netlify.app/start/?start=2nd_Floor_Parking_Garage_Entrance</v>
       </c>
       <c r="B5" t="str">
         <f>_xlfn.CONCAT(SUBSTITUTE(C4," ","_"),".png")</f>
@@ -1173,7 +1173,7 @@
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="str">
         <f t="shared" si="0"/>
-        <v>https://hospitalnavigation.netlify.app/start/?start=Rose_St_Entrance</v>
+        <v>https://uky-hospital-gps.netlify.app/start/?start=Rose_St_Entrance</v>
       </c>
       <c r="B6" t="str">
         <f t="shared" si="1"/>
@@ -1186,7 +1186,7 @@
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="str">
         <f t="shared" si="0"/>
-        <v>https://hospitalnavigation.netlify.app/start/?start=UHS_Entrance</v>
+        <v>https://uky-hospital-gps.netlify.app/start/?start=UHS_Entrance</v>
       </c>
       <c r="B7" t="str">
         <f t="shared" si="1"/>
@@ -1199,7 +1199,7 @@
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="str">
         <f t="shared" si="0"/>
-        <v>https://hospitalnavigation.netlify.app/start/?start=1st_﻿﻿﻿﻿Floor_Parking_Garage_Entrance</v>
+        <v>https://uky-hospital-gps.netlify.app/start/?start=1st_﻿﻿﻿﻿Floor_Parking_Garage_Entrance</v>
       </c>
       <c r="B8" t="str">
         <f t="shared" si="1"/>
@@ -1212,7 +1212,7 @@
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="str">
         <f t="shared" si="0"/>
-        <v>https://hospitalnavigation.netlify.app/start/?start=1st_Floor_Wing_D_Info_Desk</v>
+        <v>https://uky-hospital-gps.netlify.app/start/?start=1st_Floor_Wing_D_Info_Desk</v>
       </c>
       <c r="B9" t="str">
         <f t="shared" si="1"/>
@@ -1225,7 +1225,7 @@
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="str">
         <f t="shared" si="0"/>
-        <v>https://hospitalnavigation.netlify.app/start/?start=1st_Floor_Wing_D_South_Limestone_Entrance</v>
+        <v>https://uky-hospital-gps.netlify.app/start/?start=1st_Floor_Wing_D_South_Limestone_Entrance</v>
       </c>
       <c r="B10" t="str">
         <f t="shared" si="1"/>
@@ -1238,7 +1238,7 @@
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="str">
         <f t="shared" si="0"/>
-        <v>https://hospitalnavigation.netlify.app/start/?start=1st_Floor_Wing_D_General_Surgery_Entrance</v>
+        <v>https://uky-hospital-gps.netlify.app/start/?start=1st_Floor_Wing_D_General_Surgery_Entrance</v>
       </c>
       <c r="B11" t="str">
         <f t="shared" si="1"/>
@@ -1251,7 +1251,7 @@
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="str">
         <f t="shared" si="0"/>
-        <v>https://hospitalnavigation.netlify.app/start/?start=1st_Floor_Wing_D_North_Parking_Entrance</v>
+        <v>https://uky-hospital-gps.netlify.app/start/?start=1st_Floor_Wing_D_North_Parking_Entrance</v>
       </c>
       <c r="B12" t="str">
         <f t="shared" si="1"/>
@@ -1264,7 +1264,7 @@
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="str">
         <f t="shared" si="0"/>
-        <v>https://hospitalnavigation.netlify.app/start/?start=UHS_Bridge_Entrance</v>
+        <v>https://uky-hospital-gps.netlify.app/start/?start=UHS_Bridge_Entrance</v>
       </c>
       <c r="B13" t="str">
         <f t="shared" si="1"/>

</xml_diff>